<commit_message>
Enhance search normalization, UI, and sorting for Interview Questions and Applied Jobs. Improve link button styling and UX.
</commit_message>
<xml_diff>
--- a/backend/scraper/data/Imp1.xlsx
+++ b/backend/scraper/data/Imp1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kesha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kesha\OneDrive\Desktop\Projects\Job Automation\backend\scraper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E06658-A245-4D19-99AA-4467A79E3D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304A9A9F-25B6-43EE-96BB-0ABB60F38E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D24286F-35D7-465E-832B-7D1ED63F6A8E}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="136">
-  <si>
-    <t>Trading Firms</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="148">
   <si>
     <t>JPMC</t>
   </si>
@@ -120,9 +117,6 @@
     <t>IBM</t>
   </si>
   <si>
-    <t>UBS</t>
-  </si>
-  <si>
     <t>Two Sigma</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Intel</t>
   </si>
   <si>
-    <t>Lazard</t>
-  </si>
-  <si>
     <t>Renaissance Technologies</t>
   </si>
   <si>
@@ -201,18 +192,12 @@
     <t>VMware</t>
   </si>
   <si>
-    <t>Houlihan Lokey</t>
-  </si>
-  <si>
     <t>Point 72</t>
   </si>
   <si>
     <t>Dell</t>
   </si>
   <si>
-    <t>Greenhill &amp; Co</t>
-  </si>
-  <si>
     <t>Qube Research &amp; Technologies</t>
   </si>
   <si>
@@ -225,9 +210,6 @@
     <t>Fasanara Digital</t>
   </si>
   <si>
-    <t>Perella Weinberg</t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
@@ -258,18 +240,12 @@
     <t>Snapchat</t>
   </si>
   <si>
-    <t>JM Financial</t>
-  </si>
-  <si>
     <t>Qplum</t>
   </si>
   <si>
     <t>Dropbox</t>
   </si>
   <si>
-    <t>SBI Capital Markets</t>
-  </si>
-  <si>
     <t>iRage Capital</t>
   </si>
   <si>
@@ -291,9 +267,6 @@
     <t>Freshworks</t>
   </si>
   <si>
-    <t>Edelweiss</t>
-  </si>
-  <si>
     <t>Quadeye Securities</t>
   </si>
   <si>
@@ -309,9 +282,6 @@
     <t>Swiggy</t>
   </si>
   <si>
-    <t>ASK Capital</t>
-  </si>
-  <si>
     <t>Square Point</t>
   </si>
   <si>
@@ -336,9 +306,6 @@
     <t>BrowserStack</t>
   </si>
   <si>
-    <t>Credit Agricaole</t>
-  </si>
-  <si>
     <t>Rubrik</t>
   </si>
   <si>
@@ -442,6 +409,75 @@
   </si>
   <si>
     <t>India, Singapore, Hong Kong, London, Amsterdam, Bangalore, Mumbai, Hyderabad, Gurgaon, Gurugram</t>
+  </si>
+  <si>
+    <t>India, Bangalore, Mumbai, Hyderabad, Gurgaon, Gurugram</t>
+  </si>
+  <si>
+    <t>https://careers.bankofamerica.com/en-us/students/job-search</t>
+  </si>
+  <si>
+    <t>https://search.jobs.barclays/internships</t>
+  </si>
+  <si>
+    <t>https://careers.db.com/students-graduates/#/graduate/</t>
+  </si>
+  <si>
+    <t>https://group.bnpparibas/en/careers</t>
+  </si>
+  <si>
+    <t>https://www.lincolninternational.com/careers-and-culture/careers/students/</t>
+  </si>
+  <si>
+    <t>https://www.moelis.com/careers/</t>
+  </si>
+  <si>
+    <t>https://www.rothschildandco.com/en/careers/students-and-graduates/</t>
+  </si>
+  <si>
+    <t>https://www.evercore.com/careers/the-evercore-difference/</t>
+  </si>
+  <si>
+    <t>https://www.jefferies.com/careers/apply-now/</t>
+  </si>
+  <si>
+    <t>https://www.pjtpartners.com/careers</t>
+  </si>
+  <si>
+    <t>https://www.macquarie.com/in/en/careers/graduates-and-interns.html</t>
+  </si>
+  <si>
+    <t>https://www.kotak.com/en/about-us/careers/students-and-graduates.html</t>
+  </si>
+  <si>
+    <t>https://www.icicisecurities.com/careers/wfrmCareers.aspx</t>
+  </si>
+  <si>
+    <t>https://www.axiscapital.co.in/careers</t>
+  </si>
+  <si>
+    <t>https://careers.idfcfirstbank.com/in/en</t>
+  </si>
+  <si>
+    <t>https://www.avendus.com/india/careers/students-and-graduates</t>
+  </si>
+  <si>
+    <t>https://www.iifl.com/finance/career</t>
+  </si>
+  <si>
+    <t>https://www.nomura.com/india/careers/</t>
+  </si>
+  <si>
+    <t>https://www.hsbc.com/careers/students-and-graduates/university-students-and-graduates</t>
+  </si>
+  <si>
+    <t>https://www.sc.com/en/global-careers/experienced-hire/spotlight-career-opportunities/careers-in-india/</t>
+  </si>
+  <si>
+    <t>https://www.oppenheimer.com/careers/</t>
+  </si>
+  <si>
+    <t>https://www.equirus.com/career</t>
   </si>
 </sst>
 </file>
@@ -813,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD2321-C9BB-4C41-9B1A-F997706F310E}">
-  <dimension ref="A1:N134"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,16 +867,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -855,16 +891,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -873,16 +909,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -891,16 +927,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -909,16 +945,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -927,473 +963,537 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>74</v>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="1"/>
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F38" s="2"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F39" s="2"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F40" s="2"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F41" s="2"/>
       <c r="H41" s="2"/>
@@ -1403,1045 +1503,884 @@
         <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F42" s="2"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F43" s="2"/>
-      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="H44" s="2"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="2"/>
-      <c r="H45" s="2"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="2"/>
-      <c r="H46" s="2"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
-      </c>
-      <c r="F47" s="2"/>
-      <c r="H47" s="2"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
-      </c>
-      <c r="F48" s="2"/>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>120</v>
-      </c>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="1"/>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
-      </c>
-      <c r="F49" s="2"/>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="2"/>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
-      </c>
-      <c r="F51" s="2"/>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="2"/>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
-      </c>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>33</v>
+      </c>
       <c r="C60" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D62" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D64" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D67" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D69" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D70" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D71" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D73" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D74" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D75" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C77" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D78" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D79" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>62</v>
-      </c>
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="1"/>
       <c r="C80" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D80" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D81" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D82" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D83" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D84" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D85" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D86" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D87" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D88" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="C89" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D89" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="C90" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D90" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B91" s="1"/>
+      <c r="A91" t="s">
+        <v>34</v>
+      </c>
       <c r="C91" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D91" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C92" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D92" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C93" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D93" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C95" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D95" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C96" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C97" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D97" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D98" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C99" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D99" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C100" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D100" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C101" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D101" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C102" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D102" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C103" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D103" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C104" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D104" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C105" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D105" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C106" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D106" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C107" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D107" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C108" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D108" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C109" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D109" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C110" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D110" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C111" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D111" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="C112" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D112" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C113" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D113" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C114" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D114" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C115" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D115" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C116" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D116" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C117" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D117" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C118" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D118" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C119" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D119" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C120" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D120" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C121" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D121" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>90</v>
-      </c>
-      <c r="C122" t="s">
-        <v>132</v>
-      </c>
-      <c r="D122" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>93</v>
-      </c>
-      <c r="C123" t="s">
-        <v>132</v>
-      </c>
-      <c r="D123" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>95</v>
-      </c>
-      <c r="C124" t="s">
-        <v>132</v>
-      </c>
-      <c r="D124" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>97</v>
-      </c>
-      <c r="C125" t="s">
-        <v>132</v>
-      </c>
-      <c r="D125" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>99</v>
-      </c>
-      <c r="C126" t="s">
-        <v>132</v>
-      </c>
-      <c r="D126" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>101</v>
-      </c>
-      <c r="C127" t="s">
-        <v>132</v>
-      </c>
-      <c r="D127" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>103</v>
-      </c>
-      <c r="C128" t="s">
-        <v>132</v>
-      </c>
-      <c r="D128" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>105</v>
-      </c>
-      <c r="C129" t="s">
-        <v>132</v>
-      </c>
-      <c r="D129" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>107</v>
-      </c>
-      <c r="C130" t="s">
-        <v>132</v>
-      </c>
-      <c r="D130" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>109</v>
-      </c>
-      <c r="C131" t="s">
-        <v>132</v>
-      </c>
-      <c r="D131" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>111</v>
-      </c>
-      <c r="C132" t="s">
-        <v>132</v>
-      </c>
-      <c r="D132" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>113</v>
-      </c>
-      <c r="C133" t="s">
-        <v>132</v>
-      </c>
-      <c r="D133" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C134" t="s">
-        <v>132</v>
-      </c>
-      <c r="D134" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>